<commit_message>
docs: update learning doc
</commit_message>
<xml_diff>
--- a/learning-log.xlsx
+++ b/learning-log.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DE5561-8D4A-4C00-A9A7-CBFA3D5A16A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Branch Name</t>
   </si>
@@ -40,10 +35,25 @@
     <t>test-1</t>
   </si>
   <si>
+    <t>test-2</t>
+  </si>
+  <si>
     <t>08/03/2024</t>
   </si>
   <si>
+    <t>08/06/2024</t>
+  </si>
+  <si>
     <t>9-6</t>
+  </si>
+  <si>
+    <t>9-4:30</t>
+  </si>
+  <si>
+    <t>installation - project structure - defining routes - routes - nested routes - pages - layouts - root - layout - nested layouts - template - metadata - Link component - useRouter hook - redirect function</t>
+  </si>
+  <si>
+    <t>Suspense - loading UI - streaming with Suspense - error - global-error - redirect function - permanentRedirect function - redirect with useRouter() - redirect in next.config.js - route groups - project organization - dynamic routes - catch-all segments - parallel routes - slots - tab groups - modals - intercepting routes</t>
   </si>
   <si>
     <t>https://nextjs.org/docs/getting-started/installation
@@ -53,14 +63,14 @@
 https://nextjs.org/docs/app/building-your-application/routing/linking-and-navigating</t>
   </si>
   <si>
-    <t>installation - project structure - defining routes - routes - nested routes - pages - layouts - root - layout - nested layouts - template - metadata - Link component - useRouter hook - redirect function</t>
+    <t>https://nextjs.org/docs/app/building-your-application/routing/loading-ui-and-streaming - https://nextjs.org/docs/app/building-your-application/routing/error-handling - https://nextjs.org/docs/app/building-your-application/routing/redirecting - https://nextjs.org/docs/app/building-your-application/routing/route-groups - https://nextjs.org/docs/app/building-your-application/routing/colocation - https://nextjs.org/docs/app/building-your-application/routing/dynamic-routes - https://nextjs.org/docs/app/building-your-application/routing/parallel-routes - https://nextjs.org/docs/app/building-your-application/routing/intercepting-routes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,12 +79,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,35 +135,133 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
+      <alignment/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -147,9 +274,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +314,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -221,7 +348,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -256,10 +382,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,55 +557,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="108.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="20.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="32.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="36.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="165.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="306" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://nextjs.org/docs/getting-started/installation_x000a_https://nextjs.org/docs/getting-started/project-structure_x000a_https://nextjs.org/docs/app/building-your-application/routing/defining-routes_x000a_https://nextjs.org/docs/app/building-your-application/routing/pages-and-layouts_x000a_https://nextjs.org/docs/app/building-your-application/routing/linking-and-navigating"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://nextjs.org/docs/app/building-your-application/routing/loading-ui-and-streaming - https://nextjs.org/docs/app/building-your-application/routing/error-handling - https://nextjs.org/docs/app/building-your-application/routing/redirecting - https://nextjs.org/docs/app/building-your-application/routing/route-groups - https://nextjs.org/docs/app/building-your-application/routing/colocation - https://nextjs.org/docs/app/building-your-application/routing/dynamic-routes - https://nextjs.org/docs/app/building-your-application/routing/parallel-routes - https://nextjs.org/docs/app/building-your-application/routing/intercepting-routes"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update learning log
</commit_message>
<xml_diff>
--- a/learning-log.xlsx
+++ b/learning-log.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Next.js\next\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8570CCF-1CD3-4CF4-B311-1128673EF323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -44,12 +49,6 @@
     <t>08/06/2024</t>
   </si>
   <si>
-    <t>9-6</t>
-  </si>
-  <si>
-    <t>9-4:30</t>
-  </si>
-  <si>
     <t>installation - project structure - defining routes - routes - nested routes - pages - layouts - root - layout - nested layouts - template - metadata - Link component - useRouter hook - redirect function</t>
   </si>
   <si>
@@ -65,12 +64,18 @@
   <si>
     <t>https://nextjs.org/docs/app/building-your-application/routing/loading-ui-and-streaming - https://nextjs.org/docs/app/building-your-application/routing/error-handling - https://nextjs.org/docs/app/building-your-application/routing/redirecting - https://nextjs.org/docs/app/building-your-application/routing/route-groups - https://nextjs.org/docs/app/building-your-application/routing/colocation - https://nextjs.org/docs/app/building-your-application/routing/dynamic-routes - https://nextjs.org/docs/app/building-your-application/routing/parallel-routes - https://nextjs.org/docs/app/building-your-application/routing/intercepting-routes</t>
   </si>
+  <si>
+    <t>9 to 5</t>
+  </si>
+  <si>
+    <t>9 to 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,25 +84,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -135,133 +127,35 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
-      <alignment/>
-      <protection locked="0"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -274,9 +168,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,7 +208,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -348,6 +242,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -382,9 +277,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,23 +453,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="20.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="32.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="36.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,45 +486,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="255.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="306" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://nextjs.org/docs/getting-started/installation_x000a_https://nextjs.org/docs/getting-started/project-structure_x000a_https://nextjs.org/docs/app/building-your-application/routing/defining-routes_x000a_https://nextjs.org/docs/app/building-your-application/routing/pages-and-layouts_x000a_https://nextjs.org/docs/app/building-your-application/routing/linking-and-navigating"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://nextjs.org/docs/app/building-your-application/routing/loading-ui-and-streaming - https://nextjs.org/docs/app/building-your-application/routing/error-handling - https://nextjs.org/docs/app/building-your-application/routing/redirecting - https://nextjs.org/docs/app/building-your-application/routing/route-groups - https://nextjs.org/docs/app/building-your-application/routing/colocation - https://nextjs.org/docs/app/building-your-application/routing/dynamic-routes - https://nextjs.org/docs/app/building-your-application/routing/parallel-routes - https://nextjs.org/docs/app/building-your-application/routing/intercepting-routes"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>